<commit_message>
updates to physio data
</commit_message>
<xml_diff>
--- a/data/physiology/coli_growth_conds.xlsx
+++ b/data/physiology/coli_growth_conds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flamholz/Documents/workspace/redox-proteome/data/physiology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C86AEFE-1010-F64D-8E65-8D0F78E02A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC57A2D-2159-C540-9355-525831ECE7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36720" yWindow="-740" windowWidth="26040" windowHeight="14440" xr2:uid="{3656AAEE-C866-FA4C-8D18-91BAD9D80A7C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="70">
   <si>
     <t>c_source</t>
   </si>
@@ -191,9 +191,6 @@
     <t>decanoate</t>
   </si>
   <si>
-    <t>indole</t>
-  </si>
-  <si>
     <t>aromatic</t>
   </si>
   <si>
@@ -237,6 +234,18 @@
   </si>
   <si>
     <t>trehalose</t>
+  </si>
+  <si>
+    <t>Bergey's manual, Eschericia</t>
+  </si>
+  <si>
+    <t>phenylpropanoic acid</t>
+  </si>
+  <si>
+    <t>phenylacetic acid</t>
+  </si>
+  <si>
+    <t>3-hydroxy cinnamic acid</t>
   </si>
 </sst>
 </file>
@@ -588,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED4678C-B45E-1243-9C68-793C435C89AE}">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1554,46 +1563,72 @@
         <v>12535077</v>
       </c>
     </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C58" t="s">
         <v>9</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C59" t="s">
         <v>9</v>
       </c>
       <c r="D59">
         <v>1</v>
+      </c>
+      <c r="E59" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B60" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C60" t="s">
         <v>9</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -1601,13 +1636,16 @@
         <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C61" t="s">
         <v>9</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -1621,7 +1659,10 @@
         <v>9</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -1637,153 +1678,186 @@
       <c r="D63">
         <v>0</v>
       </c>
+      <c r="E63" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>58</v>
       </c>
       <c r="B64" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" t="s">
         <v>24</v>
       </c>
-      <c r="C64" t="s">
-        <v>9</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="C66" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B68" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>59</v>
       </c>
-      <c r="B65" t="s">
-        <v>20</v>
-      </c>
-      <c r="C65" t="s">
-        <v>9</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>18</v>
-      </c>
-      <c r="B66" t="s">
-        <v>20</v>
-      </c>
-      <c r="C66" t="s">
-        <v>9</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>31</v>
-      </c>
-      <c r="B67" t="s">
+      <c r="B69" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71" t="s">
+        <v>20</v>
+      </c>
+      <c r="C71" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73" t="s">
         <v>24</v>
       </c>
-      <c r="C67" t="s">
-        <v>9</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>32</v>
-      </c>
-      <c r="B68" t="s">
-        <v>20</v>
-      </c>
-      <c r="C68" t="s">
-        <v>9</v>
-      </c>
-      <c r="D68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>61</v>
-      </c>
-      <c r="B69" t="s">
-        <v>20</v>
-      </c>
-      <c r="C69" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>60</v>
-      </c>
-      <c r="B70" t="s">
-        <v>21</v>
-      </c>
-      <c r="C70" t="s">
-        <v>9</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>62</v>
-      </c>
-      <c r="B71" t="s">
-        <v>20</v>
-      </c>
-      <c r="C71" t="s">
-        <v>9</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>34</v>
-      </c>
-      <c r="B72" t="s">
-        <v>20</v>
-      </c>
-      <c r="C72" t="s">
-        <v>9</v>
-      </c>
-      <c r="D72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>63</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>64</v>
       </c>
-      <c r="C73" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>15</v>
-      </c>
       <c r="B74" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
@@ -1791,8 +1865,11 @@
       <c r="D74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>65</v>
       </c>
@@ -1805,47 +1882,76 @@
       <c r="D75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76" t="s">
         <v>66</v>
       </c>
-      <c r="B76" t="s">
-        <v>20</v>
-      </c>
-      <c r="C76" t="s">
-        <v>9</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B77" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <v>6345502</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78" t="s">
         <v>51</v>
-      </c>
-      <c r="B78" t="s">
-        <v>52</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78">
         <v>1</v>
+      </c>
+      <c r="E78">
+        <v>6345502</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>69</v>
+      </c>
+      <c r="B79" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>6345502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to growth modes and rates
</commit_message>
<xml_diff>
--- a/data/physiology/coli_growth_conds.xlsx
+++ b/data/physiology/coli_growth_conds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flamholz/Documents/workspace/redox-proteome/data/physiology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC57A2D-2159-C540-9355-525831ECE7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5869EE95-3C97-D646-9423-B3864A442FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36720" yWindow="-740" windowWidth="26040" windowHeight="14440" xr2:uid="{3656AAEE-C866-FA4C-8D18-91BAD9D80A7C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="83">
   <si>
     <t>c_source</t>
   </si>
@@ -246,6 +246,45 @@
   </si>
   <si>
     <t>3-hydroxy cinnamic acid</t>
+  </si>
+  <si>
+    <t>adenosine</t>
+  </si>
+  <si>
+    <t>nucleobase</t>
+  </si>
+  <si>
+    <t>PMC7527729</t>
+  </si>
+  <si>
+    <t>glucosamine</t>
+  </si>
+  <si>
+    <t>amino sugar</t>
+  </si>
+  <si>
+    <t>nucleotide</t>
+  </si>
+  <si>
+    <t>dAMP</t>
+  </si>
+  <si>
+    <t>dTMP</t>
+  </si>
+  <si>
+    <t>dGMP</t>
+  </si>
+  <si>
+    <t>dCMP</t>
+  </si>
+  <si>
+    <t>pyruvate</t>
+  </si>
+  <si>
+    <t>cysteine</t>
+  </si>
+  <si>
+    <t>threonine</t>
   </si>
 </sst>
 </file>
@@ -597,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED4678C-B45E-1243-9C68-793C435C89AE}">
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1954,6 +1993,227 @@
         <v>6345502</v>
       </c>
     </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" t="s">
+        <v>71</v>
+      </c>
+      <c r="C80" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>73</v>
+      </c>
+      <c r="B81" t="s">
+        <v>74</v>
+      </c>
+      <c r="C81" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>76</v>
+      </c>
+      <c r="B82" t="s">
+        <v>75</v>
+      </c>
+      <c r="C82" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
+        <v>35836416</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>77</v>
+      </c>
+      <c r="B83" t="s">
+        <v>75</v>
+      </c>
+      <c r="C83" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>35836416</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>78</v>
+      </c>
+      <c r="B84" t="s">
+        <v>75</v>
+      </c>
+      <c r="C84" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>35836416</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85" t="s">
+        <v>75</v>
+      </c>
+      <c r="C85" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>35836416</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>80</v>
+      </c>
+      <c r="B86" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86">
+        <v>16944129</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>40</v>
+      </c>
+      <c r="B87" t="s">
+        <v>21</v>
+      </c>
+      <c r="C87" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>16944129</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" t="s">
+        <v>21</v>
+      </c>
+      <c r="C88" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>16944129</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>28</v>
+      </c>
+      <c r="B89" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>16944129</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" t="s">
+        <v>23</v>
+      </c>
+      <c r="C90" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>35377168</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>11</v>
+      </c>
+      <c r="B91" t="s">
+        <v>23</v>
+      </c>
+      <c r="C91" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>35377168</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>82</v>
+      </c>
+      <c r="B92" t="s">
+        <v>23</v>
+      </c>
+      <c r="C92" t="s">
+        <v>9</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92">
+        <v>35377168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>